<commit_message>
complete file management methods, add workbook, sheet, fetch & private methods
</commit_message>
<xml_diff>
--- a/data/input/Book1.xlsx
+++ b/data/input/Book1.xlsx
@@ -7,21 +7,36 @@
     <workbookView xWindow="4440" yWindow="740" windowWidth="24960" windowHeight="16840"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>test</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
       <scheme val="minor"/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFFF0000"/>
+      <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
     </font>
   </fonts>
   <fills count="2">
@@ -44,8 +59,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,15 +396,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="16" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" defaultColWidth="8.83203125" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" ht="16" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
+      </c>
+      <c r="B1" s="1">
+        <f>A$1+1</f>
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>